<commit_message>
Buzzer changed from TIM9_CH1 to CH2, it's working now Pinout updated
</commit_message>
<xml_diff>
--- a/STM32F411/Pinout/MCU_pinout.xlsx
+++ b/STM32F411/Pinout/MCU_pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\RevvyDemoKit\STM32F411\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\RevvyDemoKit\STM32F411\Pinout\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -54,12 +54,6 @@
     <t>PE5</t>
   </si>
   <si>
-    <t>TIM9_CH1</t>
-  </si>
-  <si>
-    <t>BUZZER_PWM [TIM9_CH1]</t>
-  </si>
-  <si>
     <t>PE6</t>
   </si>
   <si>
@@ -691,6 +685,12 @@
   </si>
   <si>
     <t>Ultrasonic echo</t>
+  </si>
+  <si>
+    <t>TIM9_CH2</t>
+  </si>
+  <si>
+    <t>BUZZER_PWM [TIM9_CH2]</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1603,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,7 +1633,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1641,16 +1641,16 @@
         <v>92</v>
       </c>
       <c r="B2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" t="s">
         <v>198</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" t="s">
-        <v>200</v>
       </c>
       <c r="F2"/>
     </row>
@@ -1659,16 +1659,16 @@
         <v>25</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="F3" s="9"/>
     </row>
@@ -1677,34 +1677,34 @@
         <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>10</v>
+        <v>221</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>11</v>
+        <v>222</v>
       </c>
       <c r="F5" s="10"/>
     </row>
@@ -1713,19 +1713,19 @@
         <v>64</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="F6" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1733,19 +1733,19 @@
         <v>63</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="F7" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1753,16 +1753,16 @@
         <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F8"/>
     </row>
@@ -1771,16 +1771,16 @@
         <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F9"/>
     </row>
@@ -1789,16 +1789,16 @@
         <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1807,19 +1807,19 @@
         <v>81</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="F11" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1827,16 +1827,16 @@
         <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1845,16 +1845,16 @@
         <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="F13" s="12"/>
     </row>
@@ -1863,16 +1863,16 @@
         <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -1881,16 +1881,16 @@
         <v>52</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F15" s="12"/>
     </row>
@@ -1899,19 +1899,19 @@
         <v>82</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="F16" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1919,16 +1919,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -1937,16 +1937,16 @@
         <v>42</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="F18" s="12"/>
     </row>
@@ -1955,16 +1955,16 @@
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F19" s="12"/>
     </row>
@@ -1973,16 +1973,16 @@
         <v>53</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F20" s="12"/>
     </row>
@@ -1991,19 +1991,19 @@
         <v>83</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="F21" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2011,16 +2011,16 @@
         <v>78</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -2029,16 +2029,16 @@
         <v>44</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -2047,16 +2047,16 @@
         <v>79</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F24" s="12"/>
     </row>
@@ -2065,16 +2065,16 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
         <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" t="s">
-        <v>26</v>
       </c>
       <c r="F25"/>
     </row>
@@ -2083,16 +2083,16 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
         <v>27</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" t="s">
-        <v>29</v>
       </c>
       <c r="F26"/>
     </row>
@@ -2101,16 +2101,16 @@
         <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="F27" s="12"/>
     </row>
@@ -2119,19 +2119,19 @@
         <v>84</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="F28" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2139,16 +2139,16 @@
         <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F29" s="12"/>
     </row>
@@ -2157,16 +2157,16 @@
         <v>45</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="F30" s="12"/>
     </row>
@@ -2175,16 +2175,16 @@
         <v>32</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F31" s="12"/>
     </row>
@@ -2193,16 +2193,16 @@
         <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F32" s="12"/>
     </row>
@@ -2211,19 +2211,19 @@
         <v>85</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="F33" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2231,16 +2231,16 @@
         <v>68</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F34" s="12"/>
     </row>
@@ -2249,16 +2249,16 @@
         <v>77</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="F35" s="12"/>
     </row>
@@ -2267,16 +2267,16 @@
         <v>69</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F36" s="12"/>
     </row>
@@ -2285,16 +2285,16 @@
         <v>57</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F37" s="12"/>
     </row>
@@ -2303,19 +2303,19 @@
         <v>86</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="F38" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2323,16 +2323,16 @@
         <v>59</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F39" s="12"/>
     </row>
@@ -2341,16 +2341,16 @@
         <v>47</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="F40" s="12"/>
     </row>
@@ -2359,16 +2359,16 @@
         <v>60</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F41" s="12"/>
     </row>
@@ -2377,16 +2377,16 @@
         <v>15</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="F42" s="13"/>
     </row>
@@ -2395,19 +2395,19 @@
         <v>87</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>185</v>
-      </c>
       <c r="F43" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2415,19 +2415,19 @@
         <v>29</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2435,16 +2435,16 @@
         <v>16</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="F45" s="13"/>
     </row>
@@ -2453,19 +2453,19 @@
         <v>88</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="F46" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2473,19 +2473,19 @@
         <v>30</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2493,16 +2493,16 @@
         <v>17</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F48" s="13"/>
     </row>
@@ -2511,19 +2511,19 @@
         <v>55</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>113</v>
-      </c>
       <c r="F49" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2531,19 +2531,19 @@
         <v>33</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2551,16 +2551,16 @@
         <v>18</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="F51" s="13"/>
     </row>
@@ -2569,19 +2569,19 @@
         <v>56</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>116</v>
-      </c>
       <c r="F52" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2589,19 +2589,19 @@
         <v>34</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2609,16 +2609,16 @@
         <v>67</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="F54" s="13"/>
     </row>
@@ -2627,16 +2627,16 @@
         <v>66</v>
       </c>
       <c r="B55" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="F55" s="13"/>
     </row>
@@ -2645,19 +2645,19 @@
         <v>90</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="F56" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2665,19 +2665,19 @@
         <v>91</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="F57" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2685,19 +2685,19 @@
         <v>35</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="F58" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2705,19 +2705,19 @@
         <v>36</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="F59" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2725,19 +2725,19 @@
         <v>23</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="F60" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2745,19 +2745,19 @@
         <v>24</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F61" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2765,16 +2765,16 @@
         <v>76</v>
       </c>
       <c r="B62" t="s">
+        <v>152</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>153</v>
+      </c>
+      <c r="E62" t="s">
         <v>154</v>
-      </c>
-      <c r="C62" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" t="s">
-        <v>155</v>
-      </c>
-      <c r="E62" t="s">
-        <v>156</v>
       </c>
       <c r="F62"/>
     </row>
@@ -2783,16 +2783,16 @@
         <v>72</v>
       </c>
       <c r="B63" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E63" t="s">
         <v>150</v>
-      </c>
-      <c r="C63" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" t="s">
-        <v>151</v>
-      </c>
-      <c r="E63" t="s">
-        <v>152</v>
       </c>
       <c r="F63"/>
     </row>
@@ -2801,16 +2801,16 @@
         <v>89</v>
       </c>
       <c r="B64" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s">
+        <v>188</v>
+      </c>
+      <c r="E64" t="s">
         <v>189</v>
-      </c>
-      <c r="C64" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" t="s">
-        <v>190</v>
-      </c>
-      <c r="E64" t="s">
-        <v>191</v>
       </c>
       <c r="F64"/>
     </row>
@@ -2819,19 +2819,19 @@
         <v>93</v>
       </c>
       <c r="B65" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>203</v>
-      </c>
       <c r="F65" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2839,13 +2839,13 @@
         <v>96</v>
       </c>
       <c r="B66" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E66"/>
       <c r="F66"/>
@@ -2855,13 +2855,13 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E67"/>
       <c r="F67"/>
@@ -2871,13 +2871,13 @@
         <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E68"/>
       <c r="F68"/>
@@ -2926,10 +2926,10 @@
     </row>
     <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
@@ -2943,10 +2943,10 @@
         <v>6</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C73" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D73"/>
       <c r="E73"/>
@@ -2957,7 +2957,7 @@
         <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
@@ -2971,10 +2971,10 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C75" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D75"/>
       <c r="E75"/>
@@ -2985,10 +2985,10 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C76" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D76"/>
       <c r="E76"/>
@@ -2999,10 +2999,10 @@
         <v>14</v>
       </c>
       <c r="B77" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C77" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D77"/>
       <c r="E77"/>
@@ -3013,10 +3013,10 @@
         <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C78" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D78"/>
       <c r="E78"/>
@@ -3027,10 +3027,10 @@
         <v>20</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D79"/>
       <c r="E79"/>
@@ -3041,10 +3041,10 @@
         <v>21</v>
       </c>
       <c r="B80" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C80" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D80"/>
       <c r="E80"/>
@@ -3055,10 +3055,10 @@
         <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C81" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3066,10 +3066,10 @@
         <v>27</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C82" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3077,10 +3077,10 @@
         <v>28</v>
       </c>
       <c r="B83" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C83" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>37</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
@@ -3099,7 +3099,7 @@
         <v>41</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C85" t="s">
         <v>6</v>
@@ -3110,7 +3110,7 @@
         <v>43</v>
       </c>
       <c r="B86" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C86" t="s">
         <v>6</v>
@@ -3121,7 +3121,7 @@
         <v>46</v>
       </c>
       <c r="B87" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C87" t="s">
         <v>6</v>
@@ -3132,10 +3132,10 @@
         <v>48</v>
       </c>
       <c r="B88" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C88" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3143,10 +3143,10 @@
         <v>49</v>
       </c>
       <c r="B89" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C89" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3154,10 +3154,10 @@
         <v>50</v>
       </c>
       <c r="B90" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C90" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3165,7 +3165,7 @@
         <v>65</v>
       </c>
       <c r="B91" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C91" t="s">
         <v>6</v>
@@ -3176,10 +3176,10 @@
         <v>73</v>
       </c>
       <c r="B92" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C92" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3187,10 +3187,10 @@
         <v>74</v>
       </c>
       <c r="B93" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C93" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3198,10 +3198,10 @@
         <v>75</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C94" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3209,7 +3209,7 @@
         <v>80</v>
       </c>
       <c r="B95" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C95" t="s">
         <v>6</v>
@@ -3220,10 +3220,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C96" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="97" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
@@ -3242,7 +3242,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C98" t="s">
         <v>6</v>
@@ -3253,7 +3253,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C99" t="s">
         <v>6</v>
@@ -3264,10 +3264,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C100" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3275,10 +3275,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C101" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3318,7 +3318,7 @@
         <filter val="TIM4_CH2"/>
         <filter val="TIM5_CH1"/>
         <filter val="TIM5_CH2"/>
-        <filter val="TIM9_CH1"/>
+        <filter val="TIM9_CH2"/>
         <filter val="USART6_RX"/>
         <filter val="USART6_TX"/>
       </filters>
@@ -3327,7 +3327,7 @@
       <filters>
         <filter val="BAT1 [ADC_IN2]"/>
         <filter val="BAT2 [ADC_IN3]"/>
-        <filter val="BUZZER_PWM [TIM9_CH1]"/>
+        <filter val="BUZZER_PWM [TIM9_CH2]"/>
         <filter val="HM-10 [USART6 RX]"/>
         <filter val="HM-10 [USART6 TX]"/>
         <filter val="LEFT1_ENC_B"/>

</xml_diff>

<commit_message>
2018-11-14: - Schematic is now uploaded - WS2812 was unreliable with TIM+DMA, it might be a HW bug in ST's HW - WS2812 is now driven on SPI5+DMA, pin moved to PB8 from PB7 - WS2812 library contains new functions to support SPI+DMA
No patch is needed after code generation!

ToDo:
- WS2812 library cleanup is needed!
- Compass is not calibrated yet
- 6 PID controller
- USB Host?
</commit_message>
<xml_diff>
--- a/STM32F411/Pinout/MCU_pinout.xlsx
+++ b/STM32F411/Pinout/MCU_pinout.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="225">
   <si>
     <t>Position</t>
   </si>
@@ -691,13 +691,19 @@
   </si>
   <si>
     <t>BUZZER_PWM [TIM9_CH2]</t>
+  </si>
+  <si>
+    <t>SPI5_MOSI</t>
+  </si>
+  <si>
+    <t>WS2812 [SPI5_MOSI]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,6 +868,25 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1262,7 +1287,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1278,6 +1303,8 @@
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="1. jelölőszín" xfId="18" builtinId="29" customBuiltin="1"/>
@@ -1602,8 +1629,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,22 +2842,22 @@
       <c r="F64"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
+      <c r="A65" s="15">
         <v>93</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="C65" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="F65" s="10" t="s">
+      <c r="F65" s="16" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3226,18 +3253,27 @@
         <v>203</v>
       </c>
     </row>
-    <row r="97" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
         <v>95</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C97" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F97" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3247,8 +3283,11 @@
       <c r="C98" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D98"/>
+      <c r="E98"/>
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3258,8 +3297,11 @@
       <c r="C99" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D99"/>
+      <c r="E99"/>
+      <c r="F99"/>
+    </row>
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3269,8 +3311,11 @@
       <c r="C100" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="F100"/>
+    </row>
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3280,49 +3325,12 @@
       <c r="C101" t="s">
         <v>12</v>
       </c>
+      <c r="D101"/>
+      <c r="E101"/>
+      <c r="F101"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E101">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="ADC1_IN10"/>
-        <filter val="ADC1_IN11"/>
-        <filter val="ADC1_IN12"/>
-        <filter val="ADC1_IN13"/>
-        <filter val="ADC1_IN2"/>
-        <filter val="ADC1_IN3"/>
-        <filter val="GPIO_EXTI0"/>
-        <filter val="GPIO_EXTI1"/>
-        <filter val="GPIO_EXTI2"/>
-        <filter val="GPIO_EXTI3"/>
-        <filter val="GPIO_EXTI4"/>
-        <filter val="GPIO_EXTI5"/>
-        <filter val="GPIO_EXTI6"/>
-        <filter val="GPIO_EXTI7"/>
-        <filter val="GPIO_EXTI8"/>
-        <filter val="GPIO_EXTI9"/>
-        <filter val="GPIO_Input"/>
-        <filter val="GPIO_Output"/>
-        <filter val="I2C3_SCL"/>
-        <filter val="I2C3_SDA"/>
-        <filter val="TIM1_CH1"/>
-        <filter val="TIM1_CH2"/>
-        <filter val="TIM1_CH3"/>
-        <filter val="TIM1_CH4"/>
-        <filter val="TIM2_CH1"/>
-        <filter val="TIM2_CH3"/>
-        <filter val="TIM3_CH1"/>
-        <filter val="TIM3_CH2"/>
-        <filter val="TIM3_CH3"/>
-        <filter val="TIM3_CH4"/>
-        <filter val="TIM4_CH2"/>
-        <filter val="TIM5_CH1"/>
-        <filter val="TIM5_CH2"/>
-        <filter val="TIM9_CH2"/>
-        <filter val="USART6_RX"/>
-        <filter val="USART6_TX"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="4">
       <filters>
         <filter val="BAT1 [ADC_IN2]"/>
@@ -3380,6 +3388,7 @@
         <filter val="SERVO4 [TIM3_CH4]"/>
         <filter val="SERVO5 [TIM5_CH1]"/>
         <filter val="SERVO6 [TIM5_CH2]"/>
+        <filter val="WS2812 [SPI5_MOSI]"/>
         <filter val="WS2812_PWM [TIM4_CH2]"/>
       </filters>
     </filterColumn>

</xml_diff>